<commit_message>
add efs to testing px
</commit_message>
<xml_diff>
--- a/data/ewas_cpgs_top_EFS.xlsx
+++ b/data/ewas_cpgs_top_EFS.xlsx
@@ -493,7 +493,7 @@
     <t>ZMIZ1-AS1</t>
   </si>
   <si>
-    <t>PCDHGA12;PCDHGB1;PCDHGA5;PCDHGB2;PCDHGA8;PCDHGB3;PCDHGA1;PCDHGB6;PCDHGA6;PCDHGB5;PCDHGA9;PCDHGA2;PCDHGB7;PCDHGA10;PCDHGA11;PCDHGA7;PCDHGA4;PCDHGA3;PCDHGB4</t>
+    <t>PCDHGA10;PCDHGA9;PCDHGA4;PCDHGA3;PCDHGA8;PCDHGB5;PCDHGA12;PCDHGA2;PCDHGB6;PCDHGB4;PCDHGB7;PCDHGB3;PCDHGA11;PCDHGA5;PCDHGB1;PCDHGB2;PCDHGA7;PCDHGA6;PCDHGA1</t>
   </si>
   <si>
     <t>MAP2</t>
@@ -505,7 +505,7 @@
     <t>C1orf228</t>
   </si>
   <si>
-    <t>RP11-180D21.3;RP11-550P17.5</t>
+    <t>RP11-550P17.5;RP11-180D21.3</t>
   </si>
   <si>
     <t>TECPR1</t>
@@ -547,7 +547,7 @@
     <t>CYB561D1</t>
   </si>
   <si>
-    <t>PMM2;RP11-77H9.2;RP11-152P23.2</t>
+    <t>PMM2;RP11-152P23.2;RP11-77H9.2</t>
   </si>
   <si>
     <t>NLRP3</t>
@@ -583,13 +583,13 @@
     <t>TEX41</t>
   </si>
   <si>
-    <t>GSN;GSN-AS1</t>
+    <t>GSN-AS1;GSN</t>
   </si>
   <si>
     <t>MED13L</t>
   </si>
   <si>
-    <t>RP11-1021N1.1;C16orf45</t>
+    <t>C16orf45;RP11-1021N1.1</t>
   </si>
   <si>
     <t>SSH1</t>
@@ -643,7 +643,7 @@
     <t>GRXCR2</t>
   </si>
   <si>
-    <t>AC008753.6;MYADM</t>
+    <t>MYADM;AC008753.6</t>
   </si>
   <si>
     <t>TOM1L2</t>
@@ -652,7 +652,7 @@
     <t>SERINC5</t>
   </si>
   <si>
-    <t>H1FX;H1FX-AS1</t>
+    <t>H1FX-AS1;H1FX</t>
   </si>
   <si>
     <t>GNA13</t>
@@ -694,7 +694,7 @@
     <t>RAI1</t>
   </si>
   <si>
-    <t>RP11-104H15.10;FGF11;RP11-104H15.7;RP11-104H15.8</t>
+    <t>FGF11;RP11-104H15.10;RP11-104H15.7;RP11-104H15.8</t>
   </si>
   <si>
     <t>BRCA2</t>
@@ -703,7 +703,7 @@
     <t>GALNT15</t>
   </si>
   <si>
-    <t>GPR1-AS;GPR1</t>
+    <t>GPR1;GPR1-AS</t>
   </si>
   <si>
     <t>PTPRCAP;CORO1B</t>
@@ -733,7 +733,7 @@
     <t>NUDCD3</t>
   </si>
   <si>
-    <t>RNF43;BZRAP1-AS1</t>
+    <t>BZRAP1-AS1;RNF43</t>
   </si>
   <si>
     <t>protein_coding</t>
@@ -748,28 +748,28 @@
     <t>antisense</t>
   </si>
   <si>
-    <t>antisense;lincRNA</t>
+    <t>lincRNA;antisense</t>
   </si>
   <si>
     <t>lincRNA;protein_coding</t>
   </si>
   <si>
-    <t>antisense;protein_coding</t>
+    <t>protein_coding;antisense</t>
   </si>
   <si>
     <t>miRNA;transcribed_unprocessed_pseudogene</t>
   </si>
   <si>
-    <t>miRNA;protein_coding</t>
+    <t>protein_coding;miRNA</t>
   </si>
   <si>
     <t>processed_transcript</t>
   </si>
   <si>
-    <t>antisense;processed_transcript;protein_coding</t>
-  </si>
-  <si>
-    <t>processed_transcript;protein_coding</t>
+    <t>protein_coding;antisense;processed_transcript</t>
+  </si>
+  <si>
+    <t>protein_coding;processed_transcript</t>
   </si>
   <si>
     <t>N_Shelf</t>

</xml_diff>

<commit_message>
complete ewas with both risk groups
</commit_message>
<xml_diff>
--- a/data/ewas_cpgs_top_EFS.xlsx
+++ b/data/ewas_cpgs_top_EFS.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="258">
   <si>
     <t>chrm</t>
   </si>
@@ -493,7 +493,7 @@
     <t>ZMIZ1-AS1</t>
   </si>
   <si>
-    <t>PCDHGA10;PCDHGA9;PCDHGA4;PCDHGA3;PCDHGA8;PCDHGB5;PCDHGA12;PCDHGA2;PCDHGB6;PCDHGB4;PCDHGB7;PCDHGB3;PCDHGA11;PCDHGA5;PCDHGB1;PCDHGB2;PCDHGA7;PCDHGA6;PCDHGA1</t>
+    <t>PCDHGB7;PCDHGA7;PCDHGA10;PCDHGA9;PCDHGA11;PCDHGB2;PCDHGA1;PCDHGB6;PCDHGA12;PCDHGA2;PCDHGA6;PCDHGB4;PCDHGA3;PCDHGA4;PCDHGB1;PCDHGA8;PCDHGA5;PCDHGB5;PCDHGB3</t>
   </si>
   <si>
     <t>MAP2</t>
@@ -505,13 +505,13 @@
     <t>C1orf228</t>
   </si>
   <si>
-    <t>RP11-550P17.5;RP11-180D21.3</t>
+    <t>RP11-180D21.3;RP11-550P17.5</t>
   </si>
   <si>
     <t>TECPR1</t>
   </si>
   <si>
-    <t>RP5-1052I5.2;LINC01140</t>
+    <t>LINC01140;RP5-1052I5.2</t>
   </si>
   <si>
     <t>STK24</t>
@@ -547,7 +547,7 @@
     <t>CYB561D1</t>
   </si>
   <si>
-    <t>PMM2;RP11-152P23.2;RP11-77H9.2</t>
+    <t>RP11-77H9.2;RP11-152P23.2;PMM2</t>
   </si>
   <si>
     <t>NLRP3</t>
@@ -589,7 +589,7 @@
     <t>MED13L</t>
   </si>
   <si>
-    <t>C16orf45;RP11-1021N1.1</t>
+    <t>RP11-1021N1.1;C16orf45</t>
   </si>
   <si>
     <t>SSH1</t>
@@ -643,7 +643,7 @@
     <t>GRXCR2</t>
   </si>
   <si>
-    <t>MYADM;AC008753.6</t>
+    <t>AC008753.6;MYADM</t>
   </si>
   <si>
     <t>TOM1L2</t>
@@ -652,7 +652,7 @@
     <t>SERINC5</t>
   </si>
   <si>
-    <t>H1FX-AS1;H1FX</t>
+    <t>H1FX;H1FX-AS1</t>
   </si>
   <si>
     <t>GNA13</t>
@@ -694,7 +694,7 @@
     <t>RAI1</t>
   </si>
   <si>
-    <t>FGF11;RP11-104H15.10;RP11-104H15.7;RP11-104H15.8</t>
+    <t>RP11-104H15.8;FGF11;RP11-104H15.10;RP11-104H15.7</t>
   </si>
   <si>
     <t>BRCA2</t>
@@ -703,7 +703,7 @@
     <t>GALNT15</t>
   </si>
   <si>
-    <t>GPR1;GPR1-AS</t>
+    <t>GPR1-AS;GPR1</t>
   </si>
   <si>
     <t>PTPRCAP;CORO1B</t>
@@ -727,13 +727,13 @@
     <t>ROBO4</t>
   </si>
   <si>
-    <t>RP11-45M22.4;MPRIP;FLCN</t>
+    <t>MPRIP;RP11-45M22.4;FLCN</t>
   </si>
   <si>
     <t>NUDCD3</t>
   </si>
   <si>
-    <t>BZRAP1-AS1;RNF43</t>
+    <t>RNF43;BZRAP1-AS1</t>
   </si>
   <si>
     <t>protein_coding</t>
@@ -748,10 +748,10 @@
     <t>antisense</t>
   </si>
   <si>
-    <t>lincRNA;antisense</t>
-  </si>
-  <si>
-    <t>lincRNA;protein_coding</t>
+    <t>antisense;lincRNA</t>
+  </si>
+  <si>
+    <t>protein_coding;lincRNA</t>
   </si>
   <si>
     <t>protein_coding;antisense</t>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>protein_coding;miRNA</t>
+  </si>
+  <si>
+    <t>antisense;protein_coding</t>
   </si>
   <si>
     <t>processed_transcript</t>
@@ -1315,7 +1318,7 @@
         <v>150</v>
       </c>
       <c r="G4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H4">
         <v>-0.3008187042465721</v>
@@ -1415,7 +1418,7 @@
         <v>240</v>
       </c>
       <c r="G6" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H6">
         <v>-0.3915791844604438</v>
@@ -1515,7 +1518,7 @@
         <v>240</v>
       </c>
       <c r="G8" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H8">
         <v>-0.2342269749954867</v>
@@ -1615,7 +1618,7 @@
         <v>240</v>
       </c>
       <c r="G10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H10">
         <v>-0.1492697773167078</v>
@@ -1715,7 +1718,7 @@
         <v>243</v>
       </c>
       <c r="G12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H12">
         <v>-0.2375756143002867</v>
@@ -1815,7 +1818,7 @@
         <v>240</v>
       </c>
       <c r="G14" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H14">
         <v>-0.3168894735725721</v>
@@ -1965,7 +1968,7 @@
         <v>240</v>
       </c>
       <c r="G17" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H17">
         <v>1.412137953175473</v>
@@ -2015,7 +2018,7 @@
         <v>240</v>
       </c>
       <c r="G18" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H18">
         <v>-0.1634486441049782</v>
@@ -2165,7 +2168,7 @@
         <v>245</v>
       </c>
       <c r="G21" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H21">
         <v>-0.1468581147905268</v>
@@ -2215,7 +2218,7 @@
         <v>240</v>
       </c>
       <c r="G22" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H22">
         <v>-0.2254784522288338</v>
@@ -2465,7 +2468,7 @@
         <v>240</v>
       </c>
       <c r="G27" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H27">
         <v>-0.1949685263718639</v>
@@ -2565,7 +2568,7 @@
         <v>240</v>
       </c>
       <c r="G29" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H29">
         <v>-0.242658403462908</v>
@@ -2615,7 +2618,7 @@
         <v>240</v>
       </c>
       <c r="G30" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H30">
         <v>-0.2204358163601196</v>
@@ -2665,7 +2668,7 @@
         <v>150</v>
       </c>
       <c r="G31" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H31">
         <v>0.09458018232985194</v>
@@ -2815,7 +2818,7 @@
         <v>240</v>
       </c>
       <c r="G34" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H34">
         <v>-0.146611449662748</v>
@@ -2965,7 +2968,7 @@
         <v>240</v>
       </c>
       <c r="G37" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H37">
         <v>0.3674915271496308</v>
@@ -3065,7 +3068,7 @@
         <v>240</v>
       </c>
       <c r="G39" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H39">
         <v>-0.1313646291728204</v>
@@ -3315,7 +3318,7 @@
         <v>240</v>
       </c>
       <c r="G44" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H44">
         <v>-0.1206238634113921</v>
@@ -3365,7 +3368,7 @@
         <v>240</v>
       </c>
       <c r="G45" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H45">
         <v>0.2213662194953877</v>
@@ -3565,7 +3568,7 @@
         <v>150</v>
       </c>
       <c r="G49" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H49">
         <v>-0.1576899332011726</v>
@@ -3715,7 +3718,7 @@
         <v>240</v>
       </c>
       <c r="G52" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H52">
         <v>-0.104998490937256</v>
@@ -3765,7 +3768,7 @@
         <v>240</v>
       </c>
       <c r="G53" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H53">
         <v>0.2288999004485047</v>
@@ -3815,7 +3818,7 @@
         <v>248</v>
       </c>
       <c r="G54" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H54">
         <v>0.317558317553131</v>
@@ -3915,7 +3918,7 @@
         <v>240</v>
       </c>
       <c r="G56" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H56">
         <v>0.1353136177637046</v>
@@ -4315,7 +4318,7 @@
         <v>240</v>
       </c>
       <c r="G64" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H64">
         <v>-1.194255666260466</v>
@@ -4465,7 +4468,7 @@
         <v>240</v>
       </c>
       <c r="G67" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H67">
         <v>-0.3061181031857528</v>
@@ -4565,7 +4568,7 @@
         <v>240</v>
       </c>
       <c r="G69" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H69">
         <v>1.163157619480385</v>
@@ -4715,7 +4718,7 @@
         <v>150</v>
       </c>
       <c r="G72" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H72">
         <v>-0.1370354761040363</v>
@@ -4815,7 +4818,7 @@
         <v>240</v>
       </c>
       <c r="G74" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H74">
         <v>-0.2214416271415249</v>
@@ -4912,10 +4915,10 @@
         <v>209</v>
       </c>
       <c r="F76" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G76" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H76">
         <v>0.2121847828366866</v>
@@ -5115,7 +5118,7 @@
         <v>246</v>
       </c>
       <c r="G80" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H80">
         <v>0.9421416189581726</v>
@@ -5165,7 +5168,7 @@
         <v>240</v>
       </c>
       <c r="G81" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H81">
         <v>-0.2416001789830564</v>
@@ -5215,7 +5218,7 @@
         <v>240</v>
       </c>
       <c r="G82" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H82">
         <v>-0.1227144742169652</v>
@@ -5315,7 +5318,7 @@
         <v>240</v>
       </c>
       <c r="G84" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H84">
         <v>0.1404145247470952</v>
@@ -5365,7 +5368,7 @@
         <v>240</v>
       </c>
       <c r="G85" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H85">
         <v>-0.1423742317396914</v>
@@ -5415,7 +5418,7 @@
         <v>240</v>
       </c>
       <c r="G86" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H86">
         <v>0.1504752988842693</v>
@@ -5515,7 +5518,7 @@
         <v>240</v>
       </c>
       <c r="G88" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H88">
         <v>-0.1678041936356739</v>
@@ -5562,10 +5565,10 @@
         <v>221</v>
       </c>
       <c r="F89" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G89" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H89">
         <v>0.1937386830284375</v>
@@ -5665,7 +5668,7 @@
         <v>240</v>
       </c>
       <c r="G91" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H91">
         <v>0.3895085917016474</v>
@@ -5815,7 +5818,7 @@
         <v>150</v>
       </c>
       <c r="G94" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="H94">
         <v>-0.2306112443309306</v>
@@ -5915,7 +5918,7 @@
         <v>240</v>
       </c>
       <c r="G96" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="H96">
         <v>-0.2004763789903048</v>
@@ -5965,7 +5968,7 @@
         <v>240</v>
       </c>
       <c r="G97" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H97">
         <v>0.157074085352691</v>
@@ -6012,10 +6015,10 @@
         <v>226</v>
       </c>
       <c r="F98" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="G98" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H98">
         <v>0.1284849794932616</v>
@@ -6162,7 +6165,7 @@
         <v>229</v>
       </c>
       <c r="F101" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="G101" t="s">
         <v>150</v>
@@ -6215,7 +6218,7 @@
         <v>240</v>
       </c>
       <c r="G102" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H102">
         <v>0.1032718310521878</v>
@@ -6265,7 +6268,7 @@
         <v>240</v>
       </c>
       <c r="G103" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H103">
         <v>0.1213462417846451</v>
@@ -6415,7 +6418,7 @@
         <v>150</v>
       </c>
       <c r="G106" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H106">
         <v>0.1129661578912215</v>
@@ -6515,7 +6518,7 @@
         <v>240</v>
       </c>
       <c r="G108" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H108">
         <v>0.1892181922551486</v>
@@ -6762,7 +6765,7 @@
         <v>239</v>
       </c>
       <c r="F113" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="G113" t="s">
         <v>150</v>

</xml_diff>